<commit_message>
Integrated the carbon predict and made the application functional
</commit_message>
<xml_diff>
--- a/datasets/AI Energy Consumption Dataset.xlsx
+++ b/datasets/AI Energy Consumption Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Works\SustAIn\SustAIn-Backend\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECD39BD-51AE-4BB0-A794-E9F47BA55580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB313EB6-0685-4709-A529-D1D0168294DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38D89E16-535F-4CA5-8C40-947D5B651D0F}"/>
   </bookViews>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D9F9E1-76A7-4D01-8A35-934CDBDE8F96}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,8 +836,8 @@
         <v>14</v>
       </c>
       <c r="H2">
-        <f>(1750/G2)*E2</f>
-        <v>3.5926468750000002</v>
+        <f>(POWER((1750/G2),0.7)*E2)</f>
+        <v>0.84399821504019501</v>
       </c>
       <c r="I2">
         <f>(170/G2)*E2</f>
@@ -900,23 +900,23 @@
         <v>4.4206716590909094</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I3:I12" si="0">(170/G4)*E4</f>
+        <f t="shared" ref="I4:I12" si="0">(170/G4)*E4</f>
         <v>0.42943667545454545</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J3:J10" si="1">(1500/G4)*E4</f>
+        <f t="shared" ref="J4:J8" si="1">(1500/G4)*E4</f>
         <v>3.7891471363636366</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K3:K10" si="2">(200/G4)*E4</f>
+        <f t="shared" ref="K4:K10" si="2">(200/G4)*E4</f>
         <v>0.50521961818181826</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L3:L10" si="3">(70/G4)*E4</f>
+        <f t="shared" ref="L4:L10" si="3">(70/G4)*E4</f>
         <v>0.17682686636363634</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M3:M10" si="4">(13/G4)*E4</f>
+        <f t="shared" ref="M4:M10" si="4">(13/G4)*E4</f>
         <v>3.283927518181818E-2</v>
       </c>
     </row>
@@ -1005,8 +1005,7 @@
         <v>6.1209680000000001E-3</v>
       </c>
       <c r="E8">
-        <f>MAX(C58:C75)</f>
-        <v>0.17813010900000001</v>
+        <v>2.5486700000000001E-2</v>
       </c>
       <c r="F8" t="str">
         <f>_xlfn.XLOOKUP(MAX(C58:C75),C58:C75, B58:B75)</f>
@@ -1016,28 +1015,28 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H7:H12" si="5">(1750/G8)*E8</f>
-        <v>28.33888097727273</v>
+        <f t="shared" ref="H8:H12" si="5">(1750/G8)*E8</f>
+        <v>4.0547022727272726</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>2.7529198663636367</v>
+        <v>0.39388536363636367</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>24.29046940909091</v>
+        <v>3.4754590909090912</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>3.2387292545454551</v>
+        <v>0.4633945454545455</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
-        <v>1.1335552390909092</v>
+        <v>0.16218809090909092</v>
       </c>
       <c r="M8">
         <f t="shared" si="4"/>
-        <v>0.21051740154545456</v>
+        <v>3.0120645454545458E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1186,7 +1185,7 @@
       </c>
       <c r="H14">
         <f>(2.5*H2)</f>
-        <v>8.9816171875000013</v>
+        <v>2.1099955376004873</v>
       </c>
       <c r="I14">
         <f t="shared" ref="I14:M14" si="6">(2.5*I2)</f>

</xml_diff>

<commit_message>
Modified the data to represent reality more accurately
</commit_message>
<xml_diff>
--- a/datasets/AI Energy Consumption Dataset.xlsx
+++ b/datasets/AI Energy Consumption Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Works\SustAIn\SustAIn-Backend\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB313EB6-0685-4709-A529-D1D0168294DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED2EC21-1F83-4036-B2A6-EEAA87E452AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38D89E16-535F-4CA5-8C40-947D5B651D0F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
   <si>
     <t>Category</t>
   </si>
@@ -403,6 +403,12 @@
   </si>
   <si>
     <t>Max Energy of Code Generation</t>
+  </si>
+  <si>
+    <t>Formula Used :</t>
+  </si>
+  <si>
+    <t>b - efficiency gains (0.7)</t>
   </si>
 </sst>
 </file>
@@ -456,6 +462,300 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1127760</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1496307" cy="345479"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C08802B7-52BE-26DE-B338-AF9C815E66E9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14340840" y="3006090"/>
+              <a:ext cx="1496307" cy="345479"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐸</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛𝑒𝑤</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐸</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏𝑎𝑠𝑒</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>×(</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑃</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑏𝑎𝑠𝑒</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:num>
+                          <m:den>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑃</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑛𝑒𝑤</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:den>
+                        </m:f>
+                        <m:r>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>)</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-IN" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C08802B7-52BE-26DE-B338-AF9C815E66E9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14340840" y="3006090"/>
+              <a:ext cx="1496307" cy="345479"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-IN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐸_𝑛𝑒𝑤=𝐸_𝑏𝑎𝑠𝑒</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-IN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>×(〖𝑃_𝑏𝑎𝑠𝑒/𝑃_𝑛𝑒𝑤 )〗^𝑏</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-IN" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -757,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D9F9E1-76A7-4D01-8A35-934CDBDE8F96}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,7 +1070,7 @@
     <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.21875" customWidth="1"/>
     <col min="11" max="11" width="17.77734375" customWidth="1"/>
     <col min="12" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -840,24 +1140,24 @@
         <v>0.84399821504019501</v>
       </c>
       <c r="I2">
-        <f>(170/G2)*E2</f>
-        <v>0.34899998214285716</v>
+        <f>(POWER((170/G2),0.7)*E2)</f>
+        <v>0.16501717160274817</v>
       </c>
       <c r="J2">
-        <f>(1500/G2)*E2</f>
-        <v>3.0794116071428572</v>
+        <f>(POWER((1500/G2),0.7)*E2)</f>
+        <v>0.75766770364704183</v>
       </c>
       <c r="K2">
-        <f>(200/G2)*E2</f>
-        <v>0.41058821428571429</v>
+        <f>(POWER((200/G2),0.7)*E2)</f>
+        <v>0.18489956568163157</v>
       </c>
       <c r="L2">
-        <f>(70/G2)*E2</f>
-        <v>0.14370587500000001</v>
+        <f>(POWER((70/G2),0.7)*E2)</f>
+        <v>8.8671391146808859E-2</v>
       </c>
       <c r="M2">
-        <f>(13/G2)*E2</f>
-        <v>2.668823392857143E-2</v>
+        <f>(POWER((13/G2),0.7)*E2)</f>
+        <v>2.7288222070016546E-2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -896,28 +1196,28 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <f>(1750/G4)*E4</f>
-        <v>4.4206716590909094</v>
+        <f t="shared" ref="H3:H12" si="0">(POWER((1750/G4),0.7)*E4)</f>
+        <v>0.9660389790305266</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I12" si="0">(170/G4)*E4</f>
-        <v>0.42943667545454545</v>
+        <f t="shared" ref="I3:I12" si="1">(POWER((170/G4),0.7)*E4)</f>
+        <v>0.18887838521084099</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J8" si="1">(1500/G4)*E4</f>
-        <v>3.7891471363636366</v>
+        <f t="shared" ref="J3:J10" si="2">(POWER((1500/G4),0.7)*E4)</f>
+        <v>0.86722521663240049</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K10" si="2">(200/G4)*E4</f>
-        <v>0.50521961818181826</v>
+        <f t="shared" ref="K3:K10" si="3">(POWER((200/G4),0.7)*E4)</f>
+        <v>0.21163574101369942</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L10" si="3">(70/G4)*E4</f>
-        <v>0.17682686636363634</v>
+        <f t="shared" ref="L3:L10" si="4">(POWER((70/G4),0.7)*E4)</f>
+        <v>0.1014931295424603</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M10" si="4">(13/G4)*E4</f>
-        <v>3.283927518181818E-2</v>
+        <f t="shared" ref="M3:M10" si="5">(POWER((13/G4),0.7)*E4)</f>
+        <v>3.1234054430816109E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -956,28 +1256,28 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <f>(1750/G6)*E6</f>
-        <v>5.5375044772727273</v>
+        <f>(POWER((1750/G6),0.7)*E6)</f>
+        <v>1.210097827691099</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0.53792900636363639</v>
+        <f t="shared" si="1"/>
+        <v>0.23659637820289112</v>
       </c>
       <c r="J6">
-        <f t="shared" si="1"/>
-        <v>4.7464324090909091</v>
+        <f t="shared" si="2"/>
+        <v>1.086319883095161</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
-        <v>0.63285765454545462</v>
+        <f t="shared" si="3"/>
+        <v>0.26510312318813894</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
-        <v>0.22150017909090908</v>
+        <f t="shared" si="4"/>
+        <v>0.1271342236191709</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
-        <v>4.1135747545454543E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.912498588270915E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1015,28 +1315,28 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H12" si="5">(1750/G8)*E8</f>
-        <v>4.0547022727272726</v>
+        <f t="shared" si="0"/>
+        <v>0.88606454988872074</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0.39388536363636367</v>
+        <f t="shared" si="1"/>
+        <v>0.17324191363738309</v>
       </c>
       <c r="J8">
-        <f t="shared" si="1"/>
-        <v>3.4754590909090912</v>
+        <f t="shared" si="2"/>
+        <v>0.79543117607809743</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
-        <v>0.4633945454545455</v>
+        <f t="shared" si="3"/>
+        <v>0.1941152807207211</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
-        <v>0.16218809090909092</v>
+        <f t="shared" si="4"/>
+        <v>9.3090927071169421E-2</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
-        <v>3.0120645454545458E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.8648314386045433E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1075,28 +1375,28 @@
         <v>6.6</v>
       </c>
       <c r="H10">
+        <f t="shared" si="0"/>
+        <v>81.517115597209767</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>15.938095144460929</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>73.178929388525944</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>17.858425528572507</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>8.5642788260346983</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="5"/>
-        <v>434.80751151515159</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>42.238443975757576</v>
-      </c>
-      <c r="J10">
-        <f>(1500/G10)*E10</f>
-        <v>372.69215272727274</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="2"/>
-        <v>49.692287030303035</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
-        <v>17.392300460606062</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="4"/>
-        <v>3.229998656969697</v>
+        <v>2.6356183144509746</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1135,12 +1435,12 @@
         <v>9</v>
       </c>
       <c r="H12">
-        <f t="shared" si="5"/>
-        <v>0.51359894444444443</v>
+        <f t="shared" si="0"/>
+        <v>0.10567821297431479</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
-        <v>4.9892468888888888E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0662033988097666E-2</v>
       </c>
       <c r="J12" t="s">
         <v>121</v>
@@ -1189,23 +1489,23 @@
       </c>
       <c r="I14">
         <f t="shared" ref="I14:M14" si="6">(2.5*I2)</f>
-        <v>0.87249995535714286</v>
+        <v>0.41254292900687045</v>
       </c>
       <c r="J14">
         <f t="shared" si="6"/>
-        <v>7.6985290178571431</v>
+        <v>1.8941692591176045</v>
       </c>
       <c r="K14">
         <f t="shared" si="6"/>
-        <v>1.0264705357142858</v>
+        <v>0.46224891420407893</v>
       </c>
       <c r="L14">
         <f t="shared" si="6"/>
-        <v>0.35926468750000001</v>
+        <v>0.22167847786702216</v>
       </c>
       <c r="M14">
         <f t="shared" si="6"/>
-        <v>6.6720584821428577E-2</v>
+        <v>6.8220555175041359E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1230,7 +1530,7 @@
         <v>5.5938079999999996E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1241,7 +1541,7 @@
         <v>8.059587E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1251,8 +1551,11 @@
       <c r="C18">
         <v>1.943623E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1263,7 +1566,7 @@
         <v>1.9130424E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1273,8 +1576,11 @@
       <c r="C20">
         <v>2.0874859999999999E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1285,7 +1591,7 @@
         <v>1.5875393000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1296,7 +1602,7 @@
         <v>1.7333139000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1307,7 +1613,7 @@
         <v>1.6441257000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1318,7 +1624,7 @@
         <v>1.7376262999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1329,7 +1635,7 @@
         <v>2.6102442E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1340,7 +1646,7 @@
         <v>7.7082339999999996E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1351,7 +1657,7 @@
         <v>7.6446229999999997E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1362,7 +1668,7 @@
         <v>7.2795170000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1373,7 +1679,7 @@
         <v>8.0952119999999992E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1690,7 @@
         <v>8.6798110000000008E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1395,7 +1701,7 @@
         <v>1.8899583000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2267,5 +2573,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>